<commit_message>
added 1 more line, for testing purposes
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Nº</t>
   </si>
@@ -53,6 +53,15 @@
   </si>
   <si>
     <t xml:space="preserve">(0:37 - 2:37)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clara Cruz de Carvalho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/7Gbg6Z70J7E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1:42 - 3:19)</t>
   </si>
 </sst>
 </file>
@@ -191,7 +200,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -234,6 +243,10 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -316,16 +329,16 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="46.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -377,6 +390,23 @@
       </c>
       <c r="E3" s="10" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11" t="n">
+        <v>8161616209</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -384,6 +414,7 @@
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="https://youtu.be/Wa5B22KAkEk?si=C89_GNk0NGCITd32"/>
     <hyperlink ref="D3" r:id="rId2" display="https://youtu.be/bKDdT_nyP54?si=k2IXmNN2-GEZK5HB"/>
+    <hyperlink ref="D4" r:id="rId3" display="https://youtu.be/7Gbg6Z70J7E"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>